<commit_message>
Finished size metrics, started use case
</commit_message>
<xml_diff>
--- a/doc/SSRS/Metrics/SSRS_Team4_Metrics.xlsx
+++ b/doc/SSRS/Metrics/SSRS_Team4_Metrics.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="30420" yWindow="-220" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SSRS_Team4.out" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="96">
   <si>
     <t>Package</t>
   </si>
@@ -129,14 +130,212 @@
   </si>
   <si>
     <t>Lines of Code Metrics</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Use Cases Planed vs Implemented</t>
+  </si>
+  <si>
+    <t>Use Case Implemented</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Functional Requirement</t>
+  </si>
+  <si>
+    <t>See a list of open projects</t>
+  </si>
+  <si>
+    <t>Filter or search projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View more information about a specific project. </t>
+  </si>
+  <si>
+    <t>User can see a description of all of the projects avaliable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upvote and downvote projects. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment on projects and interact with its contributors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request to join a specific project. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sign up for a sQuire user account. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log in to the program using their user account. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Log out of the program using their user account. </t>
+  </si>
+  <si>
+    <t>Change their password.</t>
+  </si>
+  <si>
+    <t>Change their email.</t>
+  </si>
+  <si>
+    <t>Change their username.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open and close project chat. </t>
+  </si>
+  <si>
+    <t>We ended up leaving chat open at all times</t>
+  </si>
+  <si>
+    <t>User can see which projects he or she has been working on in the Recent Project list</t>
+  </si>
+  <si>
+    <t>Write to project chat.</t>
+  </si>
+  <si>
+    <t>Read from project chat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message a user by their name. </t>
+  </si>
+  <si>
+    <t>We had this working in a standalone chat client, but weren't able to implemented in the integrated version of the editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave a comment in a file. </t>
+  </si>
+  <si>
+    <t>A user can't leave a comment other than one that is a Java style comment in the actual file itself</t>
+  </si>
+  <si>
+    <t>Open one or more files.</t>
+  </si>
+  <si>
+    <t>Close one or more files.</t>
+  </si>
+  <si>
+    <t>Delete one or more files.</t>
+  </si>
+  <si>
+    <t>Download one or more files.</t>
+  </si>
+  <si>
+    <t>Users download files before compiling, but it is not easy to tell that this is going on</t>
+  </si>
+  <si>
+    <t>Add a new file to the project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add an existing file to the project. </t>
+  </si>
+  <si>
+    <t>We had this working in an earlier build, but ditched it when we integrated with Mobwrite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Save one or more files. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable line numbers. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable viewing reference counts above each line. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable viewing date of last edit above each line. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enable or disable view author of each line. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment/Uncomment a selected section code. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Format the document to adhere to code style. </t>
+  </si>
+  <si>
+    <t>Can only do this manually by typing //</t>
+  </si>
+  <si>
+    <t>Find/Replace specified text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">View text highlighted by other users. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type text and have the system apply syntax coloring for Java files and display errors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">View other users’ carets as they type. </t>
+  </si>
+  <si>
+    <t>Compile a project.</t>
+  </si>
+  <si>
+    <t>Execute a compiled project.</t>
+  </si>
+  <si>
+    <t>Create a new project.</t>
+  </si>
+  <si>
+    <t>Very basic here - you only really get console output</t>
+  </si>
+  <si>
+    <t>Delete a project.</t>
+  </si>
+  <si>
+    <t>Invite a user to a project.</t>
+  </si>
+  <si>
+    <t>All users can join all projects currently</t>
+  </si>
+  <si>
+    <t>Join a project.</t>
+  </si>
+  <si>
+    <t>Leave a project.</t>
+  </si>
+  <si>
+    <t>Add users to a project.</t>
+  </si>
+  <si>
+    <t>Remove users from a project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change user permissions to a project. </t>
+  </si>
+  <si>
+    <t>We decided that this was not a piece of functionallity that we wanted</t>
+  </si>
+  <si>
+    <t>Percentage Implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -161,15 +360,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -444,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,198 +1009,208 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="1">
+        <f>SUM(B33:B39)</f>
+        <v>7272</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" ref="C40:D40" si="0">SUM(C33:C39)</f>
+        <v>6559</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>713</v>
+      </c>
+      <c r="E40" s="1"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>18</v>
-      </c>
-      <c r="B42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D42" t="s">
-        <v>30</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>19</v>
-      </c>
-      <c r="B43">
-        <v>35</v>
-      </c>
-      <c r="C43">
-        <v>35</v>
-      </c>
-      <c r="D43">
-        <f>B43-C43</f>
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" t="s">
+        <v>29</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>20</v>
-      </c>
-      <c r="B44" s="1">
-        <v>2333</v>
-      </c>
-      <c r="C44" s="1">
-        <v>2233</v>
+        <v>19</v>
+      </c>
+      <c r="B44">
+        <v>35</v>
+      </c>
+      <c r="C44">
+        <v>35</v>
       </c>
       <c r="D44">
-        <f t="shared" ref="D44:D50" si="0">B44-C44</f>
-        <v>100</v>
+        <f>B44-C44</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" s="1">
-        <v>7278</v>
+        <v>2333</v>
       </c>
       <c r="C45" s="1">
-        <v>5430</v>
+        <v>2233</v>
       </c>
       <c r="D45">
-        <f t="shared" si="0"/>
-        <v>1848</v>
+        <f t="shared" ref="D45:D51" si="1">B45-C45</f>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B46" s="1">
-        <v>4783</v>
+        <v>7278</v>
       </c>
       <c r="C46" s="1">
-        <v>4761</v>
+        <v>5430</v>
       </c>
       <c r="D46">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f t="shared" si="1"/>
+        <v>1848</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47">
-        <v>29</v>
-      </c>
-      <c r="C47">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="B47" s="1">
+        <v>4783</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4761</v>
       </c>
       <c r="D47">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C48">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D48">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="1">
-        <v>4844</v>
-      </c>
-      <c r="C49" s="1">
-        <v>4844</v>
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>60</v>
+      </c>
+      <c r="C49">
+        <v>60</v>
       </c>
       <c r="D49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="1">
+        <v>4844</v>
+      </c>
+      <c r="C50" s="1">
+        <v>4844</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>26</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B51" s="1">
         <v>1087</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C51" s="1">
         <v>1087</v>
       </c>
-      <c r="D50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>33</v>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B56">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B57">
-        <v>60</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B58">
-        <v>3</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59">
         <v>3</v>
@@ -995,29 +1218,472 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B61">
-        <v>25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>26</v>
       </c>
-      <c r="B62">
+      <c r="B63">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="31" style="3" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="51.5" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="21.5" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="48" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="3">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="5">
+        <f>AVERAGE(B3:B46)</f>
+        <v>0.40909090909090912</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>